<commit_message>
Graficas y datos mes
hoja 3 del excel
</commit_message>
<xml_diff>
--- a/DB Datos.xlsx
+++ b/DB Datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\Base de datos\DolarDB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jefer\Documents\MATLAB\DolarDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D15CCC-BE37-4865-A900-5ABB8C677B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC91C84-C5E7-4E15-B219-0C74833F3A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{8B459BD6-A0E6-4669-B6A2-9CFA8FE989F0}"/>
+    <workbookView xWindow="4125" yWindow="3090" windowWidth="16200" windowHeight="9360" activeTab="1" xr2:uid="{8B459BD6-A0E6-4669-B6A2-9CFA8FE989F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>

</xml_diff>